<commit_message>
[fix] fix bug of MOU List module
</commit_message>
<xml_diff>
--- a/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
+++ b/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
   <si>
     <t>STT</t>
   </si>
@@ -106,6 +106,22 @@
     <t>SE</t>
   </si>
   <si>
+    <t>2020/1</t>
+  </si>
+  <si>
+    <t>University of Technology Sydney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/u/0/folders/1ywq6-h8okh-jcuclrgymvxg-z-q978j__x000D_
+</t>
+  </si>
+  <si>
+    <t>FGO</t>
+  </si>
+  <si>
+    <t>SE,FE</t>
+  </si>
+  <si>
     <t>2018/5</t>
   </si>
   <si>
@@ -118,12 +134,12 @@
     <t>Quản trị du lịch khách sạn</t>
   </si>
   <si>
+    <t>mauris.aliquam.eu@sedleo.net</t>
+  </si>
+  <si>
     <t>62 19 673 8307</t>
   </si>
   <si>
-    <t>FGO</t>
-  </si>
-  <si>
     <t>2018/7</t>
   </si>
   <si>
@@ -136,6 +152,9 @@
     <t>Đồ họa</t>
   </si>
   <si>
+    <t>sodales.purus@necenimNunc.edu</t>
+  </si>
+  <si>
     <t>62 33 487 6242</t>
   </si>
   <si>
@@ -154,6 +173,9 @@
     <t>Ngôn ngữ</t>
   </si>
   <si>
+    <t>non@massa.net</t>
+  </si>
+  <si>
     <t>62 39 237 3675</t>
   </si>
   <si>
@@ -169,6 +191,9 @@
     <t>Thailand</t>
   </si>
   <si>
+    <t>semper@sitametorci.com</t>
+  </si>
+  <si>
     <t>62 15 812 0688</t>
   </si>
   <si>
@@ -184,6 +209,9 @@
     <t>Ghana</t>
   </si>
   <si>
+    <t>sed.consequat@Morbiquisurna.org</t>
+  </si>
+  <si>
     <t>62 81 062 6428</t>
   </si>
   <si>
@@ -197,6 +225,9 @@
   </si>
   <si>
     <t>Malaysia</t>
+  </si>
+  <si>
+    <t>et@metusAenean.com</t>
   </si>
   <si>
     <t>62 98 631 8737</t>
@@ -219,10 +250,13 @@
     <t>Truyền thông đa phương tiện</t>
   </si>
   <si>
+    <t>sollicitudin.orci.sem@Vivamuseuismod.com</t>
+  </si>
+  <si>
     <t>05953-872277</t>
   </si>
   <si>
-    <t>2020/5</t>
+    <t>2020/6</t>
   </si>
   <si>
     <t>university of applied sciences and arts northwestern switzerland (fhnw)</t>
@@ -231,15 +265,12 @@
     <t>Switzerland</t>
   </si>
   <si>
-    <t>62 23 399 5585</t>
-  </si>
-  <si>
-    <t>2020/6</t>
-  </si>
-  <si>
     <t>Khoa học tự nhiên</t>
   </si>
   <si>
+    <t>Duis@vehiculaet.org</t>
+  </si>
+  <si>
     <t>62 55 906 2653</t>
   </si>
   <si>
@@ -255,6 +286,9 @@
     <t>Nepal</t>
   </si>
   <si>
+    <t>dictum.cursus@tortor.edu</t>
+  </si>
+  <si>
     <t>01077-046977</t>
   </si>
   <si>
@@ -267,6 +301,9 @@
     <t>India</t>
   </si>
   <si>
+    <t>cursus.purus@Praesenteu.net</t>
+  </si>
+  <si>
     <t>62 80 596 1950</t>
   </si>
   <si>
@@ -279,6 +316,9 @@
     <t>Japan</t>
   </si>
   <si>
+    <t>turpis@ut.co.uk</t>
+  </si>
+  <si>
     <t>62 89 507 3330</t>
   </si>
   <si>
@@ -291,6 +331,9 @@
     <t>Luật</t>
   </si>
   <si>
+    <t>Cum.sociis@lobortisauguescelerisque.com</t>
+  </si>
+  <si>
     <t>06201-627118</t>
   </si>
   <si>
@@ -303,6 +346,9 @@
     <t>nsg group</t>
   </si>
   <si>
+    <t>mauris.Integer.sem@felispurus.ca</t>
+  </si>
+  <si>
     <t>62 20 411 8454</t>
   </si>
   <si>
@@ -318,12 +364,18 @@
     <t>https://www.ue.edu.ph/manila/main.html?page=students&amp;link=iso</t>
   </si>
   <si>
+    <t>tellus.justo@condimentum.net</t>
+  </si>
+  <si>
     <t>62 59 735 8137</t>
   </si>
   <si>
     <t>2020/19</t>
   </si>
   <si>
+    <t>vel@congue.org</t>
+  </si>
+  <si>
     <t>62 26 323 8427</t>
   </si>
   <si>
@@ -337,6 +389,9 @@
   </si>
   <si>
     <t>www@ku.ac.th</t>
+  </si>
+  <si>
+    <t>ultricies.sem@montes.edu</t>
   </si>
   <si>
     <t>62 31 578 2509</t>
@@ -352,6 +407,9 @@
 </t>
   </si>
   <si>
+    <t>Sed.pharetra.felis@habitant.com</t>
+  </si>
+  <si>
     <t>01734-391808</t>
   </si>
   <si>
@@ -367,6 +425,9 @@
     <t>Kinh tế - quản lý</t>
   </si>
   <si>
+    <t>Proin.eget.odio@molestiesodalesMauris.edu</t>
+  </si>
+  <si>
     <t>06262-819112</t>
   </si>
   <si>
@@ -379,6 +440,9 @@
     <t>kdu university college</t>
   </si>
   <si>
+    <t>nec.diam@Sedcongueelit.ca</t>
+  </si>
+  <si>
     <t>62 45 902 2218</t>
   </si>
   <si>
@@ -388,6 +452,9 @@
     <t>the university of aizu</t>
   </si>
   <si>
+    <t>Nulla@tempor.com</t>
+  </si>
+  <si>
     <t>62 30 895 4635</t>
   </si>
   <si>
@@ -406,12 +473,18 @@
     <t>http://www.dit.ie/international/internationalnav/contactus/</t>
   </si>
   <si>
+    <t>convallis.convallis.dolor@nostraperinceptos.edu</t>
+  </si>
+  <si>
     <t>62 89 348 7901</t>
   </si>
   <si>
     <t>2020/31</t>
   </si>
   <si>
+    <t>dis@liberomauris.co.uk</t>
+  </si>
+  <si>
     <t>62 59 775 7984</t>
   </si>
   <si>
@@ -424,18 +497,27 @@
     <t>Poland</t>
   </si>
   <si>
+    <t>nec.orci.Donec@natoquepenatibus.co.uk</t>
+  </si>
+  <si>
     <t>04134-328305</t>
   </si>
   <si>
     <t>2020/36</t>
   </si>
   <si>
+    <t>Donec.porttitor@Donecnibh.co.uk</t>
+  </si>
+  <si>
     <t>06950-562167</t>
   </si>
   <si>
     <t>2020/38</t>
   </si>
   <si>
+    <t>dis.parturient@loremvehiculaet.org</t>
+  </si>
+  <si>
     <t>62 47 055 4966</t>
   </si>
   <si>
@@ -451,6 +533,9 @@
     <t>www.vu.edu.au</t>
   </si>
   <si>
+    <t>et.libero@luctus.edu</t>
+  </si>
+  <si>
     <t>62 15 171 1989</t>
   </si>
   <si>
@@ -469,7 +554,82 @@
     <t>https://drive.google.com/drive/folders/157pjfwjld1mbilckabfxodi1tcnnadd7</t>
   </si>
   <si>
+    <t>Aliquam@maurissagittis.org</t>
+  </si>
+  <si>
     <t>09762-474411</t>
+  </si>
+  <si>
+    <t>HAHA</t>
+  </si>
+  <si>
+    <t>Khoa học xã hội</t>
+  </si>
+  <si>
+    <t>d@gmail.com</t>
+  </si>
+  <si>
+    <t>0123456789</t>
+  </si>
+  <si>
+    <t>FPTUHN2</t>
+  </si>
+  <si>
+    <t>dd@</t>
+  </si>
+  <si>
+    <t>0123</t>
+  </si>
+  <si>
+    <t>SE,ME</t>
+  </si>
+  <si>
+    <t>2021/2</t>
+  </si>
+  <si>
+    <t>Khoa học tự nhiên,Khoa học xã hội</t>
+  </si>
+  <si>
+    <t>FPTUHN1</t>
+  </si>
+  <si>
+    <t>SE,FE,JR</t>
+  </si>
+  <si>
+    <t>2021/4</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>2021/5</t>
+  </si>
+  <si>
+    <t>Khoa học tự nhiên,Công nghệ thông tin,Ngôn ngữ</t>
+  </si>
+  <si>
+    <t>2021/6</t>
+  </si>
+  <si>
+    <t>Khoa học tự nhiên,Khoa học xã hội,Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>dungc843</t>
+  </si>
+  <si>
+    <t>Truong Doi</t>
+  </si>
+  <si>
+    <t>day la mot website</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>James Cook University</t>
+  </si>
+  <si>
+    <t>JC</t>
   </si>
 </sst>
 </file>
@@ -805,7 +965,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
@@ -971,25 +1131,25 @@
         <v>28</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="0">
+        <v>44175</v>
+      </c>
+      <c r="J5" s="0">
+        <v>46001</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="L5" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="I5" s="0">
-        <v>43168</v>
-      </c>
-      <c r="J5" s="0">
-        <v>44356</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6">
@@ -997,28 +1157,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>36</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>37</v>
       </c>
       <c r="I6" s="0">
-        <v>42128</v>
+        <v>43168</v>
       </c>
       <c r="J6" s="0">
-        <v>42936</v>
+        <v>44356</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>21</v>
@@ -1029,31 +1192,34 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>42</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>43</v>
       </c>
       <c r="I7" s="0">
-        <v>43150</v>
+        <v>42128</v>
       </c>
       <c r="J7" s="0">
-        <v>44520</v>
+        <v>42936</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -1070,22 +1236,25 @@
         <v>47</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="0">
+        <v>43150</v>
+      </c>
+      <c r="J8" s="0">
+        <v>44520</v>
+      </c>
+      <c r="K8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="0">
-        <v>43667</v>
-      </c>
-      <c r="J8" s="0">
-        <v>44838</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="L8" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
@@ -1093,31 +1262,34 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I9" s="0">
-        <v>43601</v>
+        <v>43667</v>
       </c>
       <c r="J9" s="0">
-        <v>44172</v>
+        <v>44838</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10">
@@ -1125,31 +1297,34 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I10" s="0">
-        <v>43781</v>
+        <v>43601</v>
       </c>
       <c r="J10" s="0">
-        <v>44915</v>
+        <v>44172</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11">
@@ -1157,34 +1332,34 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>63</v>
+        <v>35</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I11" s="0">
-        <v>44685</v>
+        <v>43781</v>
       </c>
       <c r="J11" s="0">
-        <v>45781</v>
+        <v>44915</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12">
@@ -1192,31 +1367,37 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>67</v>
+        <v>18</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>72</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>36</v>
+        <v>73</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="I12" s="0">
-        <v>44094</v>
+        <v>44685</v>
       </c>
       <c r="J12" s="0">
-        <v>45138</v>
+        <v>45781</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
@@ -1224,19 +1405,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>70</v>
+        <v>79</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="I13" s="0">
         <v>45041</v>
@@ -1245,10 +1429,10 @@
         <v>45756</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
@@ -1256,19 +1440,22 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>63</v>
+      <c r="G14" s="0" t="s">
+        <v>86</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="I14" s="0">
         <v>44147</v>
@@ -1277,7 +1464,7 @@
         <v>45364</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>26</v>
@@ -1288,19 +1475,22 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I15" s="0">
         <v>43956</v>
@@ -1312,7 +1502,7 @@
         <v>21</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
@@ -1320,19 +1510,22 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="I16" s="0">
         <v>44676</v>
@@ -1341,10 +1534,10 @@
         <v>45646</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17">
@@ -1352,19 +1545,22 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>101</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="I17" s="0">
         <v>44196</v>
@@ -1373,10 +1569,10 @@
         <v>44883</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18">
@@ -1384,19 +1580,22 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="I18" s="0">
         <v>44158</v>
@@ -1408,7 +1607,7 @@
         <v>21</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
@@ -1416,22 +1615,25 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>112</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="I19" s="0">
         <v>44033</v>
@@ -1440,10 +1642,10 @@
         <v>44434</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20">
@@ -1451,19 +1653,22 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>115</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="I20" s="0">
         <v>44311</v>
@@ -1472,10 +1677,10 @@
         <v>45280</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21">
@@ -1483,22 +1688,25 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>121</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="I21" s="0">
         <v>45407</v>
@@ -1507,10 +1715,10 @@
         <v>46491</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
@@ -1518,22 +1726,25 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="I22" s="0">
         <v>46502</v>
@@ -1542,10 +1753,10 @@
         <v>47472</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23">
@@ -1553,19 +1764,22 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>112</v>
+        <v>131</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="I23" s="0">
         <v>44016</v>
@@ -1574,10 +1788,10 @@
         <v>44586</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24">
@@ -1585,19 +1799,22 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="G24" s="0" t="s">
+        <v>137</v>
+      </c>
       <c r="H24" s="0" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="I24" s="0">
         <v>44119</v>
@@ -1606,10 +1823,10 @@
         <v>44675</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25">
@@ -1617,19 +1834,22 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>141</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="I25" s="0">
         <v>43962</v>
@@ -1641,7 +1861,7 @@
         <v>21</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26">
@@ -1649,22 +1869,25 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>70</v>
+        <v>79</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>148</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="I26" s="0">
         <v>44123</v>
@@ -1673,7 +1896,7 @@
         <v>44924</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L26" s="0" t="s">
         <v>21</v>
@@ -1684,19 +1907,22 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>151</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="I27" s="0">
         <v>45020</v>
@@ -1705,10 +1931,10 @@
         <v>45292</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28">
@@ -1716,19 +1942,22 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>156</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="I28" s="0">
         <v>44074</v>
@@ -1737,10 +1966,10 @@
         <v>44897</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29">
@@ -1748,19 +1977,22 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>159</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="I29" s="0">
         <v>45407</v>
@@ -1772,7 +2004,7 @@
         <v>21</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30">
@@ -1780,19 +2012,22 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>162</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="I30" s="0">
         <v>44655</v>
@@ -1801,10 +2036,10 @@
         <v>46619</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31">
@@ -1812,22 +2047,25 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>112</v>
+        <v>131</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>168</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="I31" s="0">
         <v>44124</v>
@@ -1836,10 +2074,10 @@
         <v>44371</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32">
@@ -1847,22 +2085,25 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>175</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="I32" s="0">
         <v>44106</v>
@@ -1874,7 +2115,278 @@
         <v>21</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>89</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>31</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="I33" s="0">
+        <v>44258</v>
+      </c>
+      <c r="J33" s="0">
+        <v>45797</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>32</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="I34" s="0">
+        <v>44265</v>
+      </c>
+      <c r="J34" s="0">
+        <v>45797</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>33</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="I35" s="0">
+        <v>43925</v>
+      </c>
+      <c r="J35" s="0">
+        <v>45748</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>34</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="I36" s="0">
+        <v>44277</v>
+      </c>
+      <c r="J36" s="0">
+        <v>44281</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>35</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="I37" s="0">
+        <v>44257</v>
+      </c>
+      <c r="J37" s="0">
+        <v>45748</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>36</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="I38" s="0">
+        <v>44259</v>
+      </c>
+      <c r="J38" s="0">
+        <v>44286</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>37</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="I39" s="0">
+        <v>44256</v>
+      </c>
+      <c r="J39" s="0">
+        <v>44286</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>38</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="I40" s="0">
+        <v>44258</v>
+      </c>
+      <c r="J40" s="0">
+        <v>44286</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[fix] fix bug of MOU module
</commit_message>
<xml_diff>
--- a/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
+++ b/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="307">
   <si>
     <t>STT</t>
   </si>
@@ -75,23 +75,50 @@
     <t>2018/1</t>
   </si>
   <si>
+    <t>James Cook University</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEVIN ANDERSON_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61 7 3001 7800_x000D_
+</t>
+  </si>
+  <si>
+    <t>31/05/2018</t>
+  </si>
+  <si>
+    <t>31/05/2021</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
     <t>Deakin University</t>
   </si>
   <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Công nghệ thông tin</t>
+    <t xml:space="preserve">JAMES K. W. LEE_x000D_
+</t>
   </si>
   <si>
     <t xml:space="preserve">61 2 9850 7111_x000D_
 </t>
   </si>
   <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>ME,SE,FE,JC</t>
+    <t>04/04/2018</t>
+  </si>
+  <si>
+    <t>SE,FE,JR,JC,ME,OJT</t>
   </si>
   <si>
     <t>Queensland University of Technology</t>
@@ -100,10 +127,17 @@
     <t>https://drive.google.com/drive/folders/1vi1sttkutztyofujf6d1wmuvs2jaxh2c</t>
   </si>
   <si>
+    <t xml:space="preserve">MR. BEN STUBBS_x000D_
+</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>SE</t>
+    <t>06/03/2018</t>
+  </si>
+  <si>
+    <t>SE,FE,JC,ME</t>
   </si>
   <si>
     <t>2020/1</t>
@@ -116,12 +150,38 @@
 </t>
   </si>
   <si>
+    <t>10/12/2020</t>
+  </si>
+  <si>
+    <t>10/12/2025</t>
+  </si>
+  <si>
     <t>FGO</t>
   </si>
   <si>
     <t>SE,FE</t>
   </si>
   <si>
+    <t>Swinburne University of Technology</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1vlnhtjyx4t0s6en0_2vghzpaakzxc9op</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM ZAHIRUL AMEEN_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">880162 7000700_x000D_
+</t>
+  </si>
+  <si>
+    <t>12/10/2020</t>
+  </si>
+  <si>
+    <t>SE,JR</t>
+  </si>
+  <si>
     <t>2018/5</t>
   </si>
   <si>
@@ -134,12 +194,24 @@
     <t>Quản trị du lịch khách sạn</t>
   </si>
   <si>
+    <t>Herman Mays</t>
+  </si>
+  <si>
     <t>mauris.aliquam.eu@sedleo.net</t>
   </si>
   <si>
     <t>62 19 673 8307</t>
   </si>
   <si>
+    <t>09/03/2018</t>
+  </si>
+  <si>
+    <t>09/06/2021</t>
+  </si>
+  <si>
+    <t>FE,ME</t>
+  </si>
+  <si>
     <t>2018/7</t>
   </si>
   <si>
@@ -152,15 +224,27 @@
     <t>Đồ họa</t>
   </si>
   <si>
+    <t>Quinlan Blanchard</t>
+  </si>
+  <si>
     <t>sodales.purus@necenimNunc.edu</t>
   </si>
   <si>
     <t>62 33 487 6242</t>
   </si>
   <si>
+    <t>04/05/2015</t>
+  </si>
+  <si>
+    <t>20/07/2017</t>
+  </si>
+  <si>
     <t>FSB</t>
   </si>
   <si>
+    <t>FE,FUS,JR</t>
+  </si>
+  <si>
     <t>2018/11</t>
   </si>
   <si>
@@ -173,12 +257,21 @@
     <t>Ngôn ngữ</t>
   </si>
   <si>
+    <t>Jasper Harper</t>
+  </si>
+  <si>
     <t>non@massa.net</t>
   </si>
   <si>
     <t>62 39 237 3675</t>
   </si>
   <si>
+    <t>19/02/2018</t>
+  </si>
+  <si>
+    <t>20/11/2021</t>
+  </si>
+  <si>
     <t>ME</t>
   </si>
   <si>
@@ -191,13 +284,22 @@
     <t>Thailand</t>
   </si>
   <si>
+    <t>Tyler Horne</t>
+  </si>
+  <si>
     <t>semper@sitametorci.com</t>
   </si>
   <si>
     <t>62 15 812 0688</t>
   </si>
   <si>
-    <t>VS</t>
+    <t>21/07/2019</t>
+  </si>
+  <si>
+    <t>04/10/2022</t>
+  </si>
+  <si>
+    <t>FE,VS</t>
   </si>
   <si>
     <t>2019/2</t>
@@ -209,13 +311,22 @@
     <t>Ghana</t>
   </si>
   <si>
+    <t>Lewis Farrell</t>
+  </si>
+  <si>
     <t>sed.consequat@Morbiquisurna.org</t>
   </si>
   <si>
     <t>62 81 062 6428</t>
   </si>
   <si>
-    <t>JTP</t>
+    <t>16/05/2019</t>
+  </si>
+  <si>
+    <t>07/12/2020</t>
+  </si>
+  <si>
+    <t>JR,JTP</t>
   </si>
   <si>
     <t>2019/18</t>
@@ -227,19 +338,25 @@
     <t>Malaysia</t>
   </si>
   <si>
+    <t>Amery Powell</t>
+  </si>
+  <si>
     <t>et@metusAenean.com</t>
   </si>
   <si>
     <t>62 98 631 8737</t>
   </si>
   <si>
-    <t>CD</t>
+    <t>12/11/2019</t>
+  </si>
+  <si>
+    <t>20/12/2022</t>
+  </si>
+  <si>
+    <t>PSE,CD,VS</t>
   </si>
   <si>
     <t>2019/20</t>
-  </si>
-  <si>
-    <t>Swinburne University of Technology</t>
   </si>
   <si>
     <t xml:space="preserve">https://drive.google.com/drive/folders/1tuqwluvlbka_vzcgkdj2olrqtfnrjqxv_x000D_
@@ -250,63 +367,129 @@
     <t>Truyền thông đa phương tiện</t>
   </si>
   <si>
+    <t>Yardley Valenzuela</t>
+  </si>
+  <si>
     <t>sollicitudin.orci.sem@Vivamuseuismod.com</t>
   </si>
   <si>
     <t>05953-872277</t>
   </si>
   <si>
+    <t>04/05/2022</t>
+  </si>
+  <si>
+    <t>04/05/2025</t>
+  </si>
+  <si>
+    <t>CD,FE</t>
+  </si>
+  <si>
+    <t>2020/5</t>
+  </si>
+  <si>
+    <t>university of applied sciences and arts northwestern switzerland (fhnw)</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Gabriel Keller</t>
+  </si>
+  <si>
+    <t>ipsum.Suspendisse.sagittis@malesuadaInteger.edu</t>
+  </si>
+  <si>
+    <t>62 23 399 5585</t>
+  </si>
+  <si>
+    <t>20/09/2020</t>
+  </si>
+  <si>
+    <t>31/07/2023</t>
+  </si>
+  <si>
+    <t>SE,FE,MUF</t>
+  </si>
+  <si>
     <t>2020/6</t>
   </si>
   <si>
-    <t>university of applied sciences and arts northwestern switzerland (fhnw)</t>
-  </si>
-  <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
     <t>Khoa học tự nhiên</t>
   </si>
   <si>
+    <t>Amery Morin</t>
+  </si>
+  <si>
     <t>Duis@vehiculaet.org</t>
   </si>
   <si>
     <t>62 55 906 2653</t>
   </si>
   <si>
+    <t>25/04/2023</t>
+  </si>
+  <si>
+    <t>09/04/2025</t>
+  </si>
+  <si>
+    <t>MUF,FE,SE</t>
+  </si>
+  <si>
+    <t>2020/8</t>
+  </si>
+  <si>
+    <t>purview education pvt. ltd.</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Bruno Melton</t>
+  </si>
+  <si>
+    <t>dictum.cursus@tortor.edu</t>
+  </si>
+  <si>
+    <t>01077-046977</t>
+  </si>
+  <si>
+    <t>12/11/2020</t>
+  </si>
+  <si>
+    <t>13/03/2024</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>2020/10</t>
+  </si>
+  <si>
+    <t>arcade institute</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Zephania Vance</t>
+  </si>
+  <si>
+    <t>cursus.purus@Praesenteu.net</t>
+  </si>
+  <si>
+    <t>62 80 596 1950</t>
+  </si>
+  <si>
+    <t>05/05/2020</t>
+  </si>
+  <si>
+    <t>22/07/2023</t>
+  </si>
+  <si>
     <t>MUF</t>
   </si>
   <si>
-    <t>2020/8</t>
-  </si>
-  <si>
-    <t>purview education pvt. ltd.</t>
-  </si>
-  <si>
-    <t>Nepal</t>
-  </si>
-  <si>
-    <t>dictum.cursus@tortor.edu</t>
-  </si>
-  <si>
-    <t>01077-046977</t>
-  </si>
-  <si>
-    <t>2020/10</t>
-  </si>
-  <si>
-    <t>arcade institute</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>cursus.purus@Praesenteu.net</t>
-  </si>
-  <si>
-    <t>62 80 596 1950</t>
-  </si>
-  <si>
     <t>2020/11</t>
   </si>
   <si>
@@ -316,12 +499,24 @@
     <t>Japan</t>
   </si>
   <si>
+    <t>Jermaine Pierce</t>
+  </si>
+  <si>
     <t>turpis@ut.co.uk</t>
   </si>
   <si>
     <t>62 89 507 3330</t>
   </si>
   <si>
+    <t>25/04/2022</t>
+  </si>
+  <si>
+    <t>20/12/2024</t>
+  </si>
+  <si>
+    <t>FUS,VS</t>
+  </si>
+  <si>
     <t>2020/12</t>
   </si>
   <si>
@@ -331,12 +526,21 @@
     <t>Luật</t>
   </si>
   <si>
+    <t>Cadman Young</t>
+  </si>
+  <si>
     <t>Cum.sociis@lobortisauguescelerisque.com</t>
   </si>
   <si>
     <t>06201-627118</t>
   </si>
   <si>
+    <t>31/12/2020</t>
+  </si>
+  <si>
+    <t>18/11/2022</t>
+  </si>
+  <si>
     <t>SA</t>
   </si>
   <si>
@@ -346,12 +550,18 @@
     <t>nsg group</t>
   </si>
   <si>
+    <t>Phelan Carver</t>
+  </si>
+  <si>
     <t>mauris.Integer.sem@felispurus.ca</t>
   </si>
   <si>
     <t>62 20 411 8454</t>
   </si>
   <si>
+    <t>23/11/2020</t>
+  </si>
+  <si>
     <t>PSE</t>
   </si>
   <si>
@@ -364,22 +574,43 @@
     <t>https://www.ue.edu.ph/manila/main.html?page=students&amp;link=iso</t>
   </si>
   <si>
+    <t>Charles Browning</t>
+  </si>
+  <si>
     <t>tellus.justo@condimentum.net</t>
   </si>
   <si>
     <t>62 59 735 8137</t>
   </si>
   <si>
+    <t>21/07/2020</t>
+  </si>
+  <si>
+    <t>26/08/2021</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
     <t>2020/19</t>
   </si>
   <si>
+    <t>Zachary Bolton</t>
+  </si>
+  <si>
     <t>vel@congue.org</t>
   </si>
   <si>
     <t>62 26 323 8427</t>
   </si>
   <si>
-    <t>JR</t>
+    <t>25/04/2021</t>
+  </si>
+  <si>
+    <t>20/12/2023</t>
+  </si>
+  <si>
+    <t>JTP,JR</t>
   </si>
   <si>
     <t>2020/20</t>
@@ -391,10 +622,22 @@
     <t>www@ku.ac.th</t>
   </si>
   <si>
+    <t>Marsden Cummings</t>
+  </si>
+  <si>
     <t>ultricies.sem@montes.edu</t>
   </si>
   <si>
     <t>62 31 578 2509</t>
+  </si>
+  <si>
+    <t>25/04/2024</t>
+  </si>
+  <si>
+    <t>14/04/2027</t>
+  </si>
+  <si>
+    <t>SA,PSE</t>
   </si>
   <si>
     <t>2020/21</t>
@@ -407,12 +650,24 @@
 </t>
   </si>
   <si>
+    <t>Noble Montgomery</t>
+  </si>
+  <si>
     <t>Sed.pharetra.felis@habitant.com</t>
   </si>
   <si>
     <t>01734-391808</t>
   </si>
   <si>
+    <t>25/04/2027</t>
+  </si>
+  <si>
+    <t>20/12/2029</t>
+  </si>
+  <si>
+    <t>JR,VS,ME</t>
+  </si>
+  <si>
     <t>2020/25</t>
   </si>
   <si>
@@ -425,13 +680,22 @@
     <t>Kinh tế - quản lý</t>
   </si>
   <si>
+    <t>Zahir Medina</t>
+  </si>
+  <si>
     <t>Proin.eget.odio@molestiesodalesMauris.edu</t>
   </si>
   <si>
     <t>06262-819112</t>
   </si>
   <si>
-    <t>SR</t>
+    <t>04/07/2020</t>
+  </si>
+  <si>
+    <t>25/01/2022</t>
+  </si>
+  <si>
+    <t>SR,SA</t>
   </si>
   <si>
     <t>2020/26</t>
@@ -440,24 +704,45 @@
     <t>kdu university college</t>
   </si>
   <si>
+    <t>Blake Mcgee</t>
+  </si>
+  <si>
     <t>nec.diam@Sedcongueelit.ca</t>
   </si>
   <si>
     <t>62 45 902 2218</t>
   </si>
   <si>
+    <t>15/10/2020</t>
+  </si>
+  <si>
+    <t>24/04/2022</t>
+  </si>
+  <si>
+    <t>JR</t>
+  </si>
+  <si>
     <t>2020/27</t>
   </si>
   <si>
     <t>the university of aizu</t>
   </si>
   <si>
+    <t>Zahir Hicks</t>
+  </si>
+  <si>
     <t>Nulla@tempor.com</t>
   </si>
   <si>
     <t>62 30 895 4635</t>
   </si>
   <si>
+    <t>11/05/2020</t>
+  </si>
+  <si>
+    <t>17/06/2021</t>
+  </si>
+  <si>
     <t>OJT</t>
   </si>
   <si>
@@ -473,21 +758,42 @@
     <t>http://www.dit.ie/international/internationalnav/contactus/</t>
   </si>
   <si>
+    <t>Dieter Huff</t>
+  </si>
+  <si>
     <t>convallis.convallis.dolor@nostraperinceptos.edu</t>
   </si>
   <si>
     <t>62 89 348 7901</t>
   </si>
   <si>
+    <t>19/10/2020</t>
+  </si>
+  <si>
+    <t>29/12/2022</t>
+  </si>
+  <si>
     <t>2020/31</t>
   </si>
   <si>
+    <t>Davis Vinson</t>
+  </si>
+  <si>
     <t>dis@liberomauris.co.uk</t>
   </si>
   <si>
     <t>62 59 775 7984</t>
   </si>
   <si>
+    <t>04/04/2023</t>
+  </si>
+  <si>
+    <t>01/01/2024</t>
+  </si>
+  <si>
+    <t>SA,SR</t>
+  </si>
+  <si>
     <t>2020/32</t>
   </si>
   <si>
@@ -497,30 +803,60 @@
     <t>Poland</t>
   </si>
   <si>
+    <t>Prescott Pickett</t>
+  </si>
+  <si>
     <t>nec.orci.Donec@natoquepenatibus.co.uk</t>
   </si>
   <si>
     <t>04134-328305</t>
   </si>
   <si>
+    <t>31/08/2020</t>
+  </si>
+  <si>
+    <t>02/12/2022</t>
+  </si>
+  <si>
     <t>2020/36</t>
   </si>
   <si>
+    <t>Hashim Nguyen</t>
+  </si>
+  <si>
     <t>Donec.porttitor@Donecnibh.co.uk</t>
   </si>
   <si>
     <t>06950-562167</t>
   </si>
   <si>
+    <t>20/12/2026</t>
+  </si>
+  <si>
+    <t>VS,CD,PSE</t>
+  </si>
+  <si>
     <t>2020/38</t>
   </si>
   <si>
+    <t>Cedric Perry</t>
+  </si>
+  <si>
     <t>dis.parturient@loremvehiculaet.org</t>
   </si>
   <si>
     <t>62 47 055 4966</t>
   </si>
   <si>
+    <t>04/04/2022</t>
+  </si>
+  <si>
+    <t>20/08/2027</t>
+  </si>
+  <si>
+    <t>ME,FE</t>
+  </si>
+  <si>
     <t>2020/40</t>
   </si>
   <si>
@@ -533,12 +869,21 @@
     <t>www.vu.edu.au</t>
   </si>
   <si>
+    <t>Valentine Meyer</t>
+  </si>
+  <si>
     <t>et.libero@luctus.edu</t>
   </si>
   <si>
     <t>62 15 171 1989</t>
   </si>
   <si>
+    <t>20/10/2020</t>
+  </si>
+  <si>
+    <t>24/06/2021</t>
+  </si>
+  <si>
     <t>SI</t>
   </si>
   <si>
@@ -554,82 +899,61 @@
     <t>https://drive.google.com/drive/folders/157pjfwjld1mbilckabfxodi1tcnnadd7</t>
   </si>
   <si>
+    <t>Elvis Walton</t>
+  </si>
+  <si>
     <t>Aliquam@maurissagittis.org</t>
   </si>
   <si>
     <t>09762-474411</t>
   </si>
   <si>
-    <t>HAHA</t>
-  </si>
-  <si>
-    <t>Khoa học xã hội</t>
-  </si>
-  <si>
-    <t>d@gmail.com</t>
+    <t>02/10/2020</t>
+  </si>
+  <si>
+    <t>03/04/2022</t>
+  </si>
+  <si>
+    <t>2000/1</t>
+  </si>
+  <si>
+    <t>Khoa học tự nhiên,Khoa học xã hội,Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>Nguyen Van A</t>
+  </si>
+  <si>
+    <t>nva@gmail.com</t>
   </si>
   <si>
     <t>0123456789</t>
   </si>
   <si>
+    <t>07/03/2000</t>
+  </si>
+  <si>
+    <t>26/03/2006</t>
+  </si>
+  <si>
     <t>FPTUHN2</t>
   </si>
   <si>
-    <t>dd@</t>
-  </si>
-  <si>
-    <t>0123</t>
-  </si>
-  <si>
-    <t>SE,ME</t>
-  </si>
-  <si>
-    <t>2021/2</t>
-  </si>
-  <si>
-    <t>Khoa học tự nhiên,Khoa học xã hội</t>
-  </si>
-  <si>
-    <t>FPTUHN1</t>
-  </si>
-  <si>
-    <t>SE,FE,JR</t>
-  </si>
-  <si>
-    <t>2021/4</t>
-  </si>
-  <si>
-    <t>sad</t>
-  </si>
-  <si>
-    <t>2021/5</t>
-  </si>
-  <si>
-    <t>Khoa học tự nhiên,Công nghệ thông tin,Ngôn ngữ</t>
-  </si>
-  <si>
-    <t>2021/6</t>
-  </si>
-  <si>
-    <t>Khoa học tự nhiên,Khoa học xã hội,Công nghệ thông tin</t>
-  </si>
-  <si>
-    <t>dungc843</t>
-  </si>
-  <si>
-    <t>Truong Doi</t>
-  </si>
-  <si>
-    <t>day la mot website</t>
-  </si>
-  <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
-    <t>James Cook University</t>
-  </si>
-  <si>
-    <t>JC</t>
+    <t>SE,FE,JR,JC</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin,Kinh tế - quản lý,Đồ họa</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn B</t>
+  </si>
+  <si>
+    <t>nvb@gmail.com</t>
+  </si>
+  <si>
+    <t>05/03/2000</t>
+  </si>
+  <si>
+    <t>JR,OJT,SA,SE</t>
   </si>
 </sst>
 </file>
@@ -674,7 +998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -965,7 +1289,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
@@ -1069,20 +1393,26 @@
       <c r="F3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="0">
-        <v>43194</v>
-      </c>
-      <c r="J3" s="0">
-        <v>44347</v>
+      <c r="I3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -1093,31 +1423,34 @@
         <v>16</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="F4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="0">
-        <v>43165</v>
-      </c>
-      <c r="J4" s="0">
-        <v>44347</v>
+      <c r="G4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -1125,31 +1458,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="0">
-        <v>44175</v>
-      </c>
-      <c r="J5" s="0">
-        <v>46001</v>
+      <c r="G5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -1157,34 +1499,34 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="0">
-        <v>43168</v>
-      </c>
-      <c r="J6" s="0">
-        <v>44356</v>
+        <v>19</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>21</v>
+        <v>42</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -1192,34 +1534,40 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>40</v>
+        <v>18</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="L7" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="0">
-        <v>42128</v>
-      </c>
-      <c r="J7" s="0">
-        <v>42936</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>21</v>
+      <c r="M7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -1227,34 +1575,40 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="0">
-        <v>43150</v>
-      </c>
-      <c r="J8" s="0">
-        <v>44520</v>
+        <v>55</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>57</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -1262,34 +1616,40 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="0">
-        <v>43667</v>
-      </c>
-      <c r="J9" s="0">
-        <v>44838</v>
+        <v>65</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10">
@@ -1297,34 +1657,40 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="0">
-        <v>43601</v>
-      </c>
-      <c r="J10" s="0">
-        <v>44172</v>
+        <v>76</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>78</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>63</v>
+        <v>42</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -1332,34 +1698,40 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="0">
-        <v>43781</v>
-      </c>
-      <c r="J11" s="0">
-        <v>44915</v>
+        <v>85</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>69</v>
+        <v>42</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -1367,37 +1739,40 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" s="0">
-        <v>44685</v>
-      </c>
-      <c r="J12" s="0">
-        <v>45781</v>
+        <v>94</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>69</v>
+        <v>24</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13">
@@ -1405,34 +1780,40 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="0">
-        <v>45041</v>
-      </c>
-      <c r="J13" s="0">
-        <v>45756</v>
+        <v>103</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>82</v>
+        <v>42</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14">
@@ -1440,34 +1821,43 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>85</v>
+        <v>18</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I14" s="0">
-        <v>44147</v>
-      </c>
-      <c r="J14" s="0">
-        <v>45364</v>
+        <v>112</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>114</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>30</v>
+        <v>115</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>26</v>
+        <v>69</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15">
@@ -1475,34 +1865,40 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" s="0">
-        <v>43956</v>
-      </c>
-      <c r="J15" s="0">
-        <v>45129</v>
+        <v>121</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>123</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>82</v>
+        <v>42</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16">
@@ -1510,34 +1906,40 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="I16" s="0">
-        <v>44676</v>
-      </c>
-      <c r="J16" s="0">
-        <v>45646</v>
+        <v>129</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>131</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>30</v>
+        <v>132</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17">
@@ -1545,34 +1947,40 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="I17" s="0">
-        <v>44196</v>
-      </c>
-      <c r="J17" s="0">
-        <v>44883</v>
+        <v>138</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>140</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>103</v>
+        <v>42</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18">
@@ -1580,34 +1988,40 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="I18" s="0">
-        <v>44158</v>
-      </c>
-      <c r="J18" s="0">
-        <v>44356</v>
+        <v>147</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>149</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>108</v>
+        <v>24</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19">
@@ -1615,37 +2029,40 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>112</v>
+        <v>155</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="I19" s="0">
-        <v>44033</v>
-      </c>
-      <c r="J19" s="0">
-        <v>44434</v>
+        <v>156</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>30</v>
+        <v>159</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>69</v>
+        <v>42</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20">
@@ -1653,34 +2070,40 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>59</v>
+        <v>162</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>60</v>
+        <v>154</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I20" s="0">
-        <v>44311</v>
-      </c>
-      <c r="J20" s="0">
-        <v>45280</v>
+        <v>165</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>167</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>117</v>
+        <v>42</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21">
@@ -1688,37 +2111,40 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="I21" s="0">
-        <v>45407</v>
-      </c>
-      <c r="J21" s="0">
-        <v>46491</v>
+        <v>173</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>175</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>108</v>
+        <v>24</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22">
@@ -1726,37 +2152,43 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>125</v>
+        <v>179</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>126</v>
+        <v>180</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I22" s="0">
-        <v>46502</v>
-      </c>
-      <c r="J22" s="0">
-        <v>47472</v>
+        <v>181</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>183</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>30</v>
+        <v>184</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>117</v>
+        <v>42</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="23">
@@ -1764,34 +2196,40 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>128</v>
+        <v>186</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>132</v>
+        <v>187</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="I23" s="0">
-        <v>44016</v>
-      </c>
-      <c r="J23" s="0">
-        <v>44586</v>
+        <v>188</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>190</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>134</v>
+        <v>42</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -1799,34 +2237,43 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>135</v>
+        <v>193</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>136</v>
+        <v>194</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>66</v>
+        <v>83</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>195</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="I24" s="0">
-        <v>44119</v>
-      </c>
-      <c r="J24" s="0">
-        <v>44675</v>
+        <v>197</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>199</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>117</v>
+        <v>42</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="25">
@@ -1834,34 +2281,43 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>139</v>
+        <v>202</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>140</v>
+        <v>203</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>204</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>141</v>
+        <v>205</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="I25" s="0">
-        <v>43962</v>
-      </c>
-      <c r="J25" s="0">
-        <v>44364</v>
+        <v>206</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>208</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>143</v>
+        <v>42</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26">
@@ -1869,37 +2325,40 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>144</v>
+        <v>211</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>145</v>
+        <v>212</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>147</v>
+        <v>213</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>79</v>
+        <v>214</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>148</v>
+        <v>215</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="I26" s="0">
-        <v>44123</v>
-      </c>
-      <c r="J26" s="0">
-        <v>44924</v>
+        <v>216</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>218</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>30</v>
+        <v>219</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>21</v>
+        <v>42</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="N26" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27">
@@ -1907,34 +2366,40 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>150</v>
+        <v>221</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>129</v>
+        <v>222</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="I27" s="0">
-        <v>45020</v>
-      </c>
-      <c r="J27" s="0">
-        <v>45292</v>
+        <v>224</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>226</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>44</v>
+        <v>227</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>103</v>
+        <v>42</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28">
@@ -1942,34 +2407,40 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>153</v>
+        <v>229</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>155</v>
-      </c>
       <c r="F28" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>156</v>
+        <v>231</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="I28" s="0">
-        <v>44074</v>
-      </c>
-      <c r="J28" s="0">
-        <v>44897</v>
+        <v>232</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>234</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>44</v>
+        <v>235</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>108</v>
+        <v>24</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="29">
@@ -1977,34 +2448,43 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>158</v>
+        <v>237</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>65</v>
+        <v>238</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>66</v>
+        <v>239</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>240</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>35</v>
+        <v>127</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>159</v>
+        <v>241</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="I29" s="0">
-        <v>45407</v>
-      </c>
-      <c r="J29" s="0">
-        <v>46376</v>
+        <v>242</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>244</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>21</v>
+        <v>245</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30">
@@ -2012,34 +2492,40 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>161</v>
+        <v>246</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>33</v>
+        <v>212</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>34</v>
+        <v>213</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>162</v>
+        <v>247</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="I30" s="0">
-        <v>44655</v>
-      </c>
-      <c r="J30" s="0">
-        <v>46619</v>
+        <v>248</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>250</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>44</v>
+        <v>251</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>51</v>
+        <v>69</v>
+      </c>
+      <c r="M30" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31">
@@ -2047,37 +2533,40 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>164</v>
+        <v>253</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>165</v>
+        <v>254</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>167</v>
+        <v>255</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>131</v>
+        <v>74</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>168</v>
+        <v>256</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="I31" s="0">
-        <v>44124</v>
-      </c>
-      <c r="J31" s="0">
-        <v>44371</v>
+        <v>257</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>259</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>30</v>
+        <v>260</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>170</v>
+        <v>69</v>
+      </c>
+      <c r="M31" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="32">
@@ -2085,37 +2574,40 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>171</v>
+        <v>261</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>172</v>
+        <v>100</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>174</v>
+        <v>101</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="I32" s="0">
-        <v>44106</v>
-      </c>
-      <c r="J32" s="0">
-        <v>44654</v>
+        <v>263</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>199</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>21</v>
+        <v>265</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>103</v>
+        <v>24</v>
+      </c>
+      <c r="M32" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="N32" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="33">
@@ -2123,34 +2615,40 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>177</v>
+        <v>267</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>178</v>
+        <v>63</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>179</v>
+        <v>268</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="I33" s="0">
-        <v>44258</v>
-      </c>
-      <c r="J33" s="0">
-        <v>45797</v>
+        <v>269</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>271</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>181</v>
+        <v>272</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>21</v>
+        <v>69</v>
+      </c>
+      <c r="M33" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="34">
@@ -2158,37 +2656,43 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>177</v>
+        <v>274</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>71</v>
+        <v>275</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>18</v>
+        <v>276</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>72</v>
+        <v>277</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>79</v>
+        <v>214</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>182</v>
+        <v>278</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I34" s="0">
-        <v>44265</v>
-      </c>
-      <c r="J34" s="0">
-        <v>45797</v>
+        <v>279</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>281</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>181</v>
+        <v>282</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>184</v>
+        <v>42</v>
+      </c>
+      <c r="M34" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="N34" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="35">
@@ -2196,28 +2700,43 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>185</v>
+        <v>284</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>17</v>
+        <v>285</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>18</v>
+        <v>286</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>287</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="I35" s="0">
-        <v>43925</v>
-      </c>
-      <c r="J35" s="0">
-        <v>45748</v>
+        <v>74</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>291</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>187</v>
+        <v>292</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>188</v>
+        <v>24</v>
+      </c>
+      <c r="M35" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="N35" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="36">
@@ -2225,34 +2744,40 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>189</v>
+        <v>293</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>186</v>
+        <v>294</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>190</v>
+        <v>295</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I36" s="0">
-        <v>44277</v>
-      </c>
-      <c r="J36" s="0">
-        <v>44281</v>
+        <v>296</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>298</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>187</v>
+        <v>299</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>31</v>
+        <v>300</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="N36" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="37">
@@ -2260,7 +2785,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>191</v>
+        <v>293</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>17</v>
@@ -2269,124 +2794,31 @@
         <v>18</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>192</v>
+        <v>302</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>303</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="I37" s="0">
-        <v>44257</v>
-      </c>
-      <c r="J37" s="0">
-        <v>45748</v>
+        <v>304</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>305</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>187</v>
+        <v>299</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="0">
-        <v>36</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="I38" s="0">
-        <v>44259</v>
-      </c>
-      <c r="J38" s="0">
-        <v>44286</v>
-      </c>
-      <c r="K38" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L38" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="0">
-        <v>37</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="I39" s="0">
-        <v>44256</v>
-      </c>
-      <c r="J39" s="0">
-        <v>44286</v>
-      </c>
-      <c r="K39" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L39" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="0">
-        <v>38</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="I40" s="0">
-        <v>44258</v>
-      </c>
-      <c r="J40" s="0">
-        <v>44286</v>
-      </c>
-      <c r="K40" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L40" s="0" t="s">
-        <v>200</v>
+        <v>300</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="N37" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[fix] change select function of MOU Code
</commit_message>
<xml_diff>
--- a/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
+++ b/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="284">
   <si>
     <t>STT</t>
   </si>
@@ -72,84 +72,22 @@
     <t>Điện thoại</t>
   </si>
   <si>
-    <t>2018/1</t>
-  </si>
-  <si>
-    <t>James Cook University</t>
+    <t>2020/1</t>
+  </si>
+  <si>
+    <t>University of Technology Sydney</t>
   </si>
   <si>
     <t>Australia</t>
-  </si>
-  <si>
-    <t>Công nghệ thông tin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KEVIN ANDERSON_x000D_
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61 7 3001 7800_x000D_
-</t>
-  </si>
-  <si>
-    <t>31/05/2018</t>
-  </si>
-  <si>
-    <t>31/05/2021</t>
-  </si>
-  <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Deakin University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAMES K. W. LEE_x000D_
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61 2 9850 7111_x000D_
-</t>
-  </si>
-  <si>
-    <t>04/04/2018</t>
-  </si>
-  <si>
-    <t>SE,FE,JR,JC,ME,OJT</t>
-  </si>
-  <si>
-    <t>Queensland University of Technology</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/1vi1sttkutztyofujf6d1wmuvs2jaxh2c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MR. BEN STUBBS_x000D_
-</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>06/03/2018</t>
-  </si>
-  <si>
-    <t>SE,FE,JC,ME</t>
-  </si>
-  <si>
-    <t>2020/1</t>
-  </si>
-  <si>
-    <t>University of Technology Sydney</t>
   </si>
   <si>
     <t xml:space="preserve">https://drive.google.com/drive/u/0/folders/1ywq6-h8okh-jcuclrgymvxg-z-q978j__x000D_
 </t>
   </si>
   <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
     <t>10/12/2020</t>
   </si>
   <si>
@@ -160,6 +98,9 @@
   </si>
   <si>
     <t>SE,FE</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
   <si>
     <t>Swinburne University of Technology</t>
@@ -324,6 +265,9 @@
   </si>
   <si>
     <t>07/12/2020</t>
+  </si>
+  <si>
+    <t>FE</t>
   </si>
   <si>
     <t>JR,JTP</t>
@@ -914,46 +858,28 @@
     <t>03/04/2022</t>
   </si>
   <si>
-    <t>2000/1</t>
-  </si>
-  <si>
-    <t>Khoa học tự nhiên,Khoa học xã hội,Công nghệ thông tin</t>
-  </si>
-  <si>
-    <t>Nguyen Van A</t>
-  </si>
-  <si>
-    <t>nva@gmail.com</t>
+    <t>2018/1</t>
+  </si>
+  <si>
+    <t>Macquarie University</t>
+  </si>
+  <si>
+    <t>Person A</t>
+  </si>
+  <si>
+    <t>a@gmail.com</t>
   </si>
   <si>
     <t>0123456789</t>
   </si>
   <si>
-    <t>07/03/2000</t>
-  </si>
-  <si>
-    <t>26/03/2006</t>
-  </si>
-  <si>
-    <t>FPTUHN2</t>
-  </si>
-  <si>
-    <t>SE,FE,JR,JC</t>
-  </si>
-  <si>
-    <t>Công nghệ thông tin,Kinh tế - quản lý,Đồ họa</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn B</t>
-  </si>
-  <si>
-    <t>nvb@gmail.com</t>
-  </si>
-  <si>
-    <t>05/03/2000</t>
-  </si>
-  <si>
-    <t>JR,OJT,SA,SE</t>
+    <t>01/03/2018</t>
+  </si>
+  <si>
+    <t>31/05/2021</t>
+  </si>
+  <si>
+    <t>SE,JTP,SI</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1215,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
@@ -1390,23 +1316,20 @@
       <c r="D3" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="F3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>24</v>
@@ -1428,26 +1351,29 @@
       <c r="D4" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="E4" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="F4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="M4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N4" s="0" t="s">
         <v>25</v>
@@ -1458,37 +1384,37 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="M5" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="N5" s="0" t="s">
         <v>25</v>
@@ -1499,31 +1425,37 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="N6" s="0" t="s">
         <v>25</v>
@@ -1534,37 +1466,37 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>46</v>
+        <v>57</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="N7" s="0" t="s">
         <v>25</v>
@@ -1575,37 +1507,37 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="N8" s="0" t="s">
         <v>25</v>
@@ -1616,37 +1548,37 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="N9" s="0" t="s">
         <v>25</v>
@@ -1657,37 +1589,37 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="N10" s="0" t="s">
         <v>25</v>
@@ -1698,37 +1630,40 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>83</v>
+        <v>18</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>92</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="N11" s="0" t="s">
         <v>25</v>
@@ -1739,37 +1674,37 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="N12" s="0" t="s">
         <v>25</v>
@@ -1780,37 +1715,37 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="N13" s="0" t="s">
         <v>25</v>
@@ -1821,40 +1756,37 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="N14" s="0" t="s">
         <v>25</v>
@@ -1865,37 +1797,37 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="N15" s="0" t="s">
         <v>25</v>
@@ -1906,37 +1838,37 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="N16" s="0" t="s">
         <v>25</v>
@@ -1947,37 +1879,37 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="N17" s="0" t="s">
         <v>25</v>
@@ -1988,37 +1920,37 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="N18" s="0" t="s">
         <v>25</v>
@@ -2029,37 +1961,40 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>154</v>
+        <v>44</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>162</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="N19" s="0" t="s">
         <v>25</v>
@@ -2070,37 +2005,37 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>154</v>
+        <v>74</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="N20" s="0" t="s">
         <v>25</v>
@@ -2111,37 +2046,40 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>154</v>
+        <v>65</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>178</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>58</v>
+        <v>183</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="N21" s="0" t="s">
         <v>25</v>
@@ -2152,40 +2090,40 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="N22" s="0" t="s">
         <v>25</v>
@@ -2196,37 +2134,37 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>91</v>
+        <v>195</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>92</v>
+        <v>196</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="N23" s="0" t="s">
         <v>25</v>
@@ -2237,40 +2175,37 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>195</v>
+        <v>84</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="N24" s="0" t="s">
         <v>25</v>
@@ -2281,40 +2216,37 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>204</v>
+        <v>137</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="N25" s="0" t="s">
         <v>25</v>
@@ -2325,37 +2257,40 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>213</v>
+        <v>222</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>223</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>214</v>
+        <v>110</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>220</v>
+        <v>80</v>
       </c>
       <c r="N26" s="0" t="s">
         <v>25</v>
@@ -2366,37 +2301,37 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="N27" s="0" t="s">
         <v>25</v>
@@ -2407,37 +2342,37 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>236</v>
+        <v>159</v>
       </c>
       <c r="N28" s="0" t="s">
         <v>25</v>
@@ -2448,40 +2383,37 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>238</v>
+        <v>83</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>240</v>
+        <v>84</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>244</v>
+        <v>182</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
       <c r="N29" s="0" t="s">
         <v>25</v>
@@ -2492,37 +2424,37 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>212</v>
+        <v>33</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>213</v>
+        <v>34</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="N30" s="0" t="s">
         <v>25</v>
@@ -2533,37 +2465,40 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>260</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>74</v>
+        <v>197</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>176</v>
+        <v>266</v>
       </c>
       <c r="N31" s="0" t="s">
         <v>25</v>
@@ -2574,37 +2509,40 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>100</v>
+        <v>268</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>101</v>
+        <v>269</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>270</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>199</v>
+        <v>274</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>266</v>
+        <v>152</v>
       </c>
       <c r="N32" s="0" t="s">
         <v>25</v>
@@ -2615,209 +2553,39 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>51</v>
+        <v>277</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="0">
-        <v>32</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="L34" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="M34" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="N34" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="0">
-        <v>33</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="J35" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="K35" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="L35" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M35" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="N35" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="0">
-        <v>34</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="K36" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="L36" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="M36" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="N36" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="0">
-        <v>35</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="K37" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="L37" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="M37" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="N37" s="0" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[add, fix] - add export function list partner, deleted partner, fix list deleted mou datatable css
</commit_message>
<xml_diff>
--- a/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
+++ b/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t>STT</t>
   </si>
@@ -72,37 +72,447 @@
     <t>Điện thoại</t>
   </si>
   <si>
-    <t>2021/1</t>
+    <t>2018/1</t>
+  </si>
+  <si>
+    <t>James Cook University</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Khoa học xã hội,Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>KEVIN ANDERSON</t>
+  </si>
+  <si>
+    <t>61 7 3001 7800</t>
+  </si>
+  <si>
+    <t>31/05/2018</t>
+  </si>
+  <si>
+    <t>31/05/2021</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>PSE</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>2015/1</t>
   </si>
   <si>
     <t>Macquarie University</t>
   </si>
   <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Khoa học xã hội</t>
-  </si>
-  <si>
-    <t>Kiểm tra MOU</t>
-  </si>
-  <si>
-    <t>0123456789</t>
-  </si>
-  <si>
-    <t>08/04/2020</t>
-  </si>
-  <si>
-    <t>22/04/2025</t>
-  </si>
-  <si>
-    <t>FPTUHN1</t>
+    <t>Công nghệ thông tin,Ngôn ngữ</t>
+  </si>
+  <si>
+    <t>JAMES K. W. LEE</t>
+  </si>
+  <si>
+    <t>61 2 9850 7111</t>
+  </si>
+  <si>
+    <t>07/07/2015</t>
+  </si>
+  <si>
+    <t>14/04/2020</t>
+  </si>
+  <si>
+    <t>SE,JC,ME,SI</t>
+  </si>
+  <si>
+    <t>2015/2</t>
+  </si>
+  <si>
+    <t>Deakin University</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Khoa học tự nhiên,Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>MR. BEN STUBBS</t>
+  </si>
+  <si>
+    <t>03/07/2015</t>
+  </si>
+  <si>
+    <t>03/07/2020</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>2016/1</t>
+  </si>
+  <si>
+    <t>University of Technology Sydney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/u/0/folders/1ywq6-h8okh-jcuclrgymvxg-z-q978j__x000D_
+</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>WILLIAM PURCELL</t>
+  </si>
+  <si>
+    <t>SIMON.WATSON@UTS.EDU.AU</t>
+  </si>
+  <si>
+    <t>61 2 9514 2589</t>
+  </si>
+  <si>
+    <t>18/01/2016</t>
+  </si>
+  <si>
+    <t>18/01/2021</t>
+  </si>
+  <si>
+    <t>SE,SA</t>
+  </si>
+  <si>
+    <t>2018/2</t>
+  </si>
+  <si>
+    <t>Swinburne University of Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1tuqwluvlbka_vzcgkdj2olrqtfnrjqxv_x000D_
+_x000D_
+</t>
+  </si>
+  <si>
+    <t>01/10/2018</t>
+  </si>
+  <si>
+    <t>01/10/2021</t>
+  </si>
+  <si>
+    <t>FGO</t>
+  </si>
+  <si>
+    <t>2019/1</t>
+  </si>
+  <si>
+    <t>Queensland University of Technology</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1vi1sttkutztyofujf6d1wmuvs2jaxh2c</t>
+  </si>
+  <si>
+    <t>03/09/2019</t>
+  </si>
+  <si>
+    <t>03/09/2022</t>
+  </si>
+  <si>
+    <t>2020/1</t>
+  </si>
+  <si>
+    <t>10/12/2020</t>
+  </si>
+  <si>
+    <t>10/12/2025</t>
+  </si>
+  <si>
+    <t>SE,FE</t>
+  </si>
+  <si>
+    <t>2017/1</t>
+  </si>
+  <si>
+    <t>Glee Education</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>KM ZAHIRUL AMEEN</t>
+  </si>
+  <si>
+    <t>INFFOGLEEBD@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>880162 7000700</t>
+  </si>
+  <si>
+    <t>24/11/2017</t>
+  </si>
+  <si>
+    <t>31/12/2020</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>2016/2</t>
+  </si>
+  <si>
+    <t>Greybites Consultlants</t>
+  </si>
+  <si>
+    <t>Khoa học tự nhiên,Khoa học xã hội</t>
+  </si>
+  <si>
+    <t>06/01/2016</t>
+  </si>
+  <si>
+    <t>05/01/2017</t>
+  </si>
+  <si>
+    <t>2013/1</t>
+  </si>
+  <si>
+    <t>Global Immigration Consultants Ltd.</t>
+  </si>
+  <si>
+    <t>https://www.ue.edu.ph/manila/main.html?page=students&amp;link=iso</t>
+  </si>
+  <si>
+    <t>SALMAN OMAR</t>
+  </si>
+  <si>
+    <t>S.OMAR@GICBD.COM</t>
+  </si>
+  <si>
+    <t>88 0177 8000400</t>
+  </si>
+  <si>
+    <t>13/08/2013</t>
+  </si>
+  <si>
+    <t>13/08/2014</t>
+  </si>
+  <si>
+    <t>2013/2</t>
+  </si>
+  <si>
+    <t>Fair International</t>
+  </si>
+  <si>
+    <t>M.A. SALAM SAJIB</t>
+  </si>
+  <si>
+    <t>FAIRINTERNATIONAL_BD_71@YAHOO.COM</t>
+  </si>
+  <si>
+    <t>88 02 8157433</t>
+  </si>
+  <si>
+    <t>01/05/2013</t>
+  </si>
+  <si>
+    <t>30/04/2014</t>
+  </si>
+  <si>
+    <t>2013/3</t>
+  </si>
+  <si>
+    <t>Euro Education Fair</t>
+  </si>
+  <si>
+    <t>MD. KAMRUL ISLAM</t>
+  </si>
+  <si>
+    <t>2015/3</t>
+  </si>
+  <si>
+    <t>Artevelde University College Ghent</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Khoa học xã hội,Ngôn ngữ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DR. JOHAN VEEKMAN </t>
+  </si>
+  <si>
+    <t>SEVERINE.VANDERSTIGHELEN@ARTEVELDEHS.BE</t>
+  </si>
+  <si>
+    <t>32 9 234 90 64</t>
+  </si>
+  <si>
+    <t>20/08/2015</t>
+  </si>
+  <si>
+    <t>20/08/2018</t>
+  </si>
+  <si>
+    <t>SE,FE,JR,CD</t>
+  </si>
+  <si>
+    <t>2013/4</t>
+  </si>
+  <si>
+    <t>Universiti Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>http://www.ubd.edu.bn/menu/service-and-administration/student-affairs-section/international-student-office/</t>
+  </si>
+  <si>
+    <t>ANITA AZIZ</t>
+  </si>
+  <si>
+    <t>02/07/2013</t>
+  </si>
+  <si>
+    <t>02/07/2016</t>
+  </si>
+  <si>
+    <t>SE,FE,JR,JC,ME</t>
+  </si>
+  <si>
+    <t>2018/3</t>
+  </si>
+  <si>
+    <t>DR. JOYCE TEO SIEW YEAN</t>
+  </si>
+  <si>
+    <t>26/02/2018</t>
+  </si>
+  <si>
+    <t>31/10/2018</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>2019/2</t>
+  </si>
+  <si>
+    <t>Universiti Teknologi Brunei</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/12iEPuJzmk6Ausqjz8aOZJyrFoY1hDto5</t>
+  </si>
+  <si>
+    <t>17/04/2019</t>
+  </si>
+  <si>
+    <t>14/04/2024</t>
+  </si>
+  <si>
+    <t>2015/4</t>
+  </si>
+  <si>
+    <t>Zaman University</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>DR. ERKAN POLATDEMIR</t>
+  </si>
+  <si>
+    <t>info@zamanu.edu.kh</t>
+  </si>
+  <si>
+    <t>855 23 996 111</t>
+  </si>
+  <si>
+    <t>17/04/2015</t>
+  </si>
+  <si>
+    <t>2019/3</t>
+  </si>
+  <si>
+    <t>Universiti Teknologi Petronas</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1p876oqt_paeysyfj974yrojfxo0drk91_x000D_
+</t>
+  </si>
+  <si>
+    <t>04/04/2019</t>
+  </si>
+  <si>
+    <t>04/04/2022</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>2015/5</t>
+  </si>
+  <si>
+    <t>Kyoto University of Foreign Studies</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ,Kinh tế - quản lý</t>
+  </si>
+  <si>
+    <t>YOSHIKAZU MORITA</t>
+  </si>
+  <si>
+    <t>OIPS@KUFS.AC.JP</t>
+  </si>
+  <si>
+    <t>81 75 322 6043</t>
+  </si>
+  <si>
+    <t>12/09/2015</t>
+  </si>
+  <si>
+    <t>12/09/2016</t>
+  </si>
+  <si>
+    <t>2019/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyoto Computer Gakuin_x000D_
+ - The Kyoto College of Graduate Studies for Information</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1qjyjdgmbgkmrftj6n-0cpynrsewytwkz</t>
+  </si>
+  <si>
+    <t>09/03/2019</t>
+  </si>
+  <si>
+    <t>09/03/2024</t>
+  </si>
+  <si>
+    <t>2018/4</t>
+  </si>
+  <si>
+    <t>Ural Federal University</t>
+  </si>
+  <si>
+    <t>Russian Federation (the)</t>
+  </si>
+  <si>
+    <t>26/12/2018</t>
+  </si>
+  <si>
+    <t>26/12/2022</t>
   </si>
   <si>
     <t>FE,SE</t>
-  </si>
-  <si>
-    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -438,7 +848,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
@@ -545,9 +955,6 @@
       <c r="G3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="I3" s="0" t="s">
         <v>21</v>
       </c>
@@ -565,6 +972,760 @@
       </c>
       <c r="N3" s="0" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>15</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>16</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>17</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>20</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>21</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[add, fix] - add export function list partner, deleted partner, fix list deleted mou datatable css (#1062)
</commit_message>
<xml_diff>
--- a/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
+++ b/MANAGER/Content/assets/excel/Collaboration/Download/MOU.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t>STT</t>
   </si>
@@ -72,37 +72,447 @@
     <t>Điện thoại</t>
   </si>
   <si>
-    <t>2021/1</t>
+    <t>2018/1</t>
+  </si>
+  <si>
+    <t>James Cook University</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Khoa học xã hội,Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>KEVIN ANDERSON</t>
+  </si>
+  <si>
+    <t>61 7 3001 7800</t>
+  </si>
+  <si>
+    <t>31/05/2018</t>
+  </si>
+  <si>
+    <t>31/05/2021</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>PSE</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>2015/1</t>
   </si>
   <si>
     <t>Macquarie University</t>
   </si>
   <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Khoa học xã hội</t>
-  </si>
-  <si>
-    <t>Kiểm tra MOU</t>
-  </si>
-  <si>
-    <t>0123456789</t>
-  </si>
-  <si>
-    <t>08/04/2020</t>
-  </si>
-  <si>
-    <t>22/04/2025</t>
-  </si>
-  <si>
-    <t>FPTUHN1</t>
+    <t>Công nghệ thông tin,Ngôn ngữ</t>
+  </si>
+  <si>
+    <t>JAMES K. W. LEE</t>
+  </si>
+  <si>
+    <t>61 2 9850 7111</t>
+  </si>
+  <si>
+    <t>07/07/2015</t>
+  </si>
+  <si>
+    <t>14/04/2020</t>
+  </si>
+  <si>
+    <t>SE,JC,ME,SI</t>
+  </si>
+  <si>
+    <t>2015/2</t>
+  </si>
+  <si>
+    <t>Deakin University</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Khoa học tự nhiên,Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>MR. BEN STUBBS</t>
+  </si>
+  <si>
+    <t>03/07/2015</t>
+  </si>
+  <si>
+    <t>03/07/2020</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>2016/1</t>
+  </si>
+  <si>
+    <t>University of Technology Sydney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/u/0/folders/1ywq6-h8okh-jcuclrgymvxg-z-q978j__x000D_
+</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>WILLIAM PURCELL</t>
+  </si>
+  <si>
+    <t>SIMON.WATSON@UTS.EDU.AU</t>
+  </si>
+  <si>
+    <t>61 2 9514 2589</t>
+  </si>
+  <si>
+    <t>18/01/2016</t>
+  </si>
+  <si>
+    <t>18/01/2021</t>
+  </si>
+  <si>
+    <t>SE,SA</t>
+  </si>
+  <si>
+    <t>2018/2</t>
+  </si>
+  <si>
+    <t>Swinburne University of Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1tuqwluvlbka_vzcgkdj2olrqtfnrjqxv_x000D_
+_x000D_
+</t>
+  </si>
+  <si>
+    <t>01/10/2018</t>
+  </si>
+  <si>
+    <t>01/10/2021</t>
+  </si>
+  <si>
+    <t>FGO</t>
+  </si>
+  <si>
+    <t>2019/1</t>
+  </si>
+  <si>
+    <t>Queensland University of Technology</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1vi1sttkutztyofujf6d1wmuvs2jaxh2c</t>
+  </si>
+  <si>
+    <t>03/09/2019</t>
+  </si>
+  <si>
+    <t>03/09/2022</t>
+  </si>
+  <si>
+    <t>2020/1</t>
+  </si>
+  <si>
+    <t>10/12/2020</t>
+  </si>
+  <si>
+    <t>10/12/2025</t>
+  </si>
+  <si>
+    <t>SE,FE</t>
+  </si>
+  <si>
+    <t>2017/1</t>
+  </si>
+  <si>
+    <t>Glee Education</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>KM ZAHIRUL AMEEN</t>
+  </si>
+  <si>
+    <t>INFFOGLEEBD@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>880162 7000700</t>
+  </si>
+  <si>
+    <t>24/11/2017</t>
+  </si>
+  <si>
+    <t>31/12/2020</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>2016/2</t>
+  </si>
+  <si>
+    <t>Greybites Consultlants</t>
+  </si>
+  <si>
+    <t>Khoa học tự nhiên,Khoa học xã hội</t>
+  </si>
+  <si>
+    <t>06/01/2016</t>
+  </si>
+  <si>
+    <t>05/01/2017</t>
+  </si>
+  <si>
+    <t>2013/1</t>
+  </si>
+  <si>
+    <t>Global Immigration Consultants Ltd.</t>
+  </si>
+  <si>
+    <t>https://www.ue.edu.ph/manila/main.html?page=students&amp;link=iso</t>
+  </si>
+  <si>
+    <t>SALMAN OMAR</t>
+  </si>
+  <si>
+    <t>S.OMAR@GICBD.COM</t>
+  </si>
+  <si>
+    <t>88 0177 8000400</t>
+  </si>
+  <si>
+    <t>13/08/2013</t>
+  </si>
+  <si>
+    <t>13/08/2014</t>
+  </si>
+  <si>
+    <t>2013/2</t>
+  </si>
+  <si>
+    <t>Fair International</t>
+  </si>
+  <si>
+    <t>M.A. SALAM SAJIB</t>
+  </si>
+  <si>
+    <t>FAIRINTERNATIONAL_BD_71@YAHOO.COM</t>
+  </si>
+  <si>
+    <t>88 02 8157433</t>
+  </si>
+  <si>
+    <t>01/05/2013</t>
+  </si>
+  <si>
+    <t>30/04/2014</t>
+  </si>
+  <si>
+    <t>2013/3</t>
+  </si>
+  <si>
+    <t>Euro Education Fair</t>
+  </si>
+  <si>
+    <t>MD. KAMRUL ISLAM</t>
+  </si>
+  <si>
+    <t>2015/3</t>
+  </si>
+  <si>
+    <t>Artevelde University College Ghent</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Khoa học xã hội,Ngôn ngữ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DR. JOHAN VEEKMAN </t>
+  </si>
+  <si>
+    <t>SEVERINE.VANDERSTIGHELEN@ARTEVELDEHS.BE</t>
+  </si>
+  <si>
+    <t>32 9 234 90 64</t>
+  </si>
+  <si>
+    <t>20/08/2015</t>
+  </si>
+  <si>
+    <t>20/08/2018</t>
+  </si>
+  <si>
+    <t>SE,FE,JR,CD</t>
+  </si>
+  <si>
+    <t>2013/4</t>
+  </si>
+  <si>
+    <t>Universiti Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>http://www.ubd.edu.bn/menu/service-and-administration/student-affairs-section/international-student-office/</t>
+  </si>
+  <si>
+    <t>ANITA AZIZ</t>
+  </si>
+  <si>
+    <t>02/07/2013</t>
+  </si>
+  <si>
+    <t>02/07/2016</t>
+  </si>
+  <si>
+    <t>SE,FE,JR,JC,ME</t>
+  </si>
+  <si>
+    <t>2018/3</t>
+  </si>
+  <si>
+    <t>DR. JOYCE TEO SIEW YEAN</t>
+  </si>
+  <si>
+    <t>26/02/2018</t>
+  </si>
+  <si>
+    <t>31/10/2018</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>2019/2</t>
+  </si>
+  <si>
+    <t>Universiti Teknologi Brunei</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/12iEPuJzmk6Ausqjz8aOZJyrFoY1hDto5</t>
+  </si>
+  <si>
+    <t>17/04/2019</t>
+  </si>
+  <si>
+    <t>14/04/2024</t>
+  </si>
+  <si>
+    <t>2015/4</t>
+  </si>
+  <si>
+    <t>Zaman University</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>DR. ERKAN POLATDEMIR</t>
+  </si>
+  <si>
+    <t>info@zamanu.edu.kh</t>
+  </si>
+  <si>
+    <t>855 23 996 111</t>
+  </si>
+  <si>
+    <t>17/04/2015</t>
+  </si>
+  <si>
+    <t>2019/3</t>
+  </si>
+  <si>
+    <t>Universiti Teknologi Petronas</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1p876oqt_paeysyfj974yrojfxo0drk91_x000D_
+</t>
+  </si>
+  <si>
+    <t>04/04/2019</t>
+  </si>
+  <si>
+    <t>04/04/2022</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>2015/5</t>
+  </si>
+  <si>
+    <t>Kyoto University of Foreign Studies</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ,Kinh tế - quản lý</t>
+  </si>
+  <si>
+    <t>YOSHIKAZU MORITA</t>
+  </si>
+  <si>
+    <t>OIPS@KUFS.AC.JP</t>
+  </si>
+  <si>
+    <t>81 75 322 6043</t>
+  </si>
+  <si>
+    <t>12/09/2015</t>
+  </si>
+  <si>
+    <t>12/09/2016</t>
+  </si>
+  <si>
+    <t>2019/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyoto Computer Gakuin_x000D_
+ - The Kyoto College of Graduate Studies for Information</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1qjyjdgmbgkmrftj6n-0cpynrsewytwkz</t>
+  </si>
+  <si>
+    <t>09/03/2019</t>
+  </si>
+  <si>
+    <t>09/03/2024</t>
+  </si>
+  <si>
+    <t>2018/4</t>
+  </si>
+  <si>
+    <t>Ural Federal University</t>
+  </si>
+  <si>
+    <t>Russian Federation (the)</t>
+  </si>
+  <si>
+    <t>26/12/2018</t>
+  </si>
+  <si>
+    <t>26/12/2022</t>
   </si>
   <si>
     <t>FE,SE</t>
-  </si>
-  <si>
-    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -438,7 +848,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
@@ -545,9 +955,6 @@
       <c r="G3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="I3" s="0" t="s">
         <v>21</v>
       </c>
@@ -565,6 +972,760 @@
       </c>
       <c r="N3" s="0" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>15</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>16</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>17</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>20</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>21</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>